<commit_message>
mudanças na apresentação dos resultados
</commit_message>
<xml_diff>
--- a/001-random-vpl-model/results/Results.xlsx
+++ b/001-random-vpl-model/results/Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DADOS\dev\exploratory-models\001-model-01\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DADOS\dev\exploratory-models\001-random-vpl-model\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -389,13 +389,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>